<commit_message>
Updated results spreadsheet with default xgboost results and sequential SHA results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\IdeaProjects\751-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84946BF5-EBCB-4E0B-93A6-DC158D28779B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F21344-9449-445B-8C90-99499A7FEF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F301625-1DEF-4B5B-95C7-F7A21235A7CE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
   <si>
     <t>Random Search</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Score</t>
-  </si>
-  <si>
-    <t>SHA</t>
   </si>
   <si>
     <t>Configs</t>
@@ -98,6 +95,15 @@
   </si>
   <si>
     <t>Max_Samples</t>
+  </si>
+  <si>
+    <t>SHA (Sequential)</t>
+  </si>
+  <si>
+    <t>SHA (4 Workers)</t>
+  </si>
+  <si>
+    <t>Default XGBoost</t>
   </si>
 </sst>
 </file>
@@ -237,16 +243,143 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.0570525752979984E-2"/>
+          <c:y val="7.8120166295811769E-2"/>
+          <c:w val="0.91326795605498001"/>
+          <c:h val="0.76537518372701474"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$13</c:f>
+              <c:f>'All Comparisons'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'All Comparisons'!$B$7:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.1829504990000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0321923569999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.175202556999899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.707698913999899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.854793258999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.513741218999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173.930542304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>347.405843667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>646.110279770999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Comparisons'!$C$7:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.81897465652677304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81897465652677304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82661424571640396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.829446683641195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83464635318708902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83464635318708902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83990634314602997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84158649364433302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84158649364433302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D95-497C-8CDB-F6FFA836C081}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'All Comparisons'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -281,7 +414,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$B$15:$B$19</c:f>
+              <c:f>'All Comparisons'!$B$19:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -305,7 +438,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$C$15:$C$19</c:f>
+              <c:f>'All Comparisons'!$C$19:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -335,15 +468,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:idx val="6"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$1</c:f>
+              <c:f>'All Comparisons'!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Random Search</c:v>
+                  <c:v>SHA (Sequential)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -351,7 +484,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -362,11 +497,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -374,72 +513,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$B$3:$B$11</c:f>
+              <c:f>'All Comparisons'!$E$28:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.1829504990000004</c:v>
+                  <c:v>7.8567875279999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0321923569999996</c:v>
+                  <c:v>18.032700009999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.175202556999899</c:v>
+                  <c:v>54.981309652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.707698913999899</c:v>
+                  <c:v>130.196151867</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.854793258999997</c:v>
+                  <c:v>316.754186562999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.513741218999996</c:v>
+                  <c:v>638.44272856099997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>173.930542304</c:v>
+                  <c:v>1366.714942757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347.405843667</c:v>
+                  <c:v>3076.4089409479998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>646.110279770999</c:v>
+                  <c:v>6800.0111336159998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14686.297701968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$C$3:$C$11</c:f>
+              <c:f>'All Comparisons'!$F$28:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.81897465652677304</c:v>
+                  <c:v>0.83857121633142395</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81897465652677304</c:v>
+                  <c:v>0.84106500452140698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82661424571640396</c:v>
+                  <c:v>0.85510070225260804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.829446683641195</c:v>
+                  <c:v>0.85827123062081301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83464635318708902</c:v>
+                  <c:v>0.86166429233839203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83464635318708902</c:v>
+                  <c:v>0.86476990517609498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83990634314602997</c:v>
+                  <c:v>0.86679088244786895</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.84158649364433302</c:v>
+                  <c:v>0.86589166383800498</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.84158649364433302</c:v>
+                  <c:v>0.86505731151354803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.86591944234864904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,20 +592,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D95-497C-8CDB-F6FFA836C081}"/>
+              <c16:uniqueId val="{00000000-3724-4D20-A866-A59A7E5B24B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$22</c:f>
+              <c:f>'All Comparisons'!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SHA</c:v>
+                  <c:v>SHA (4 Workers)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -491,7 +636,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$E$24:$E$33</c:f>
+              <c:f>'All Comparisons'!$E$44:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -530,7 +675,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$24:$F$33</c:f>
+              <c:f>'All Comparisons'!$F$44:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -576,10 +721,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$35</c:f>
+              <c:f>'All Comparisons'!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -614,7 +759,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$37:$F$46</c:f>
+              <c:f>'All Comparisons'!$F$57:$F$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -653,7 +798,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$G$37:$G$46</c:f>
+              <c:f>'All Comparisons'!$G$57:$G$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -699,10 +844,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$48</c:f>
+              <c:f>'All Comparisons'!$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -737,7 +882,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$50:$F$59</c:f>
+              <c:f>'All Comparisons'!$F$70:$F$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -776,7 +921,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$G$50:$G$59</c:f>
+              <c:f>'All Comparisons'!$G$70:$G$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -822,10 +967,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$61</c:f>
+              <c:f>'All Comparisons'!$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -860,7 +1005,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$63:$F$72</c:f>
+              <c:f>'All Comparisons'!$F$83:$F$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -899,7 +1044,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$G$63:$G$72</c:f>
+              <c:f>'All Comparisons'!$G$83:$G$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1081,6 +1226,7 @@
         <c:axId val="707966784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.87000000000000011"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1193,6 +1339,7 @@
         <c:crossAx val="707965800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-3"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1353,16 +1500,143 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8726531235001415E-2"/>
+          <c:y val="9.9603883393319284E-2"/>
+          <c:w val="0.90518997248112665"/>
+          <c:h val="0.74389146662950711"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$13</c:f>
+              <c:f>'All Comparisons'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'All Comparisons'!$B$7:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.1829504990000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0321923569999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.175202556999899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.707698913999899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.854793258999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.513741218999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173.930542304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>347.405843667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>646.110279770999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Comparisons'!$A$7:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F9B-47E1-A228-AD326CCFD2E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'All Comparisons'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1397,7 +1671,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$B$15:$B$19</c:f>
+              <c:f>'All Comparisons'!$B$19:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1421,7 +1695,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$D$15:$D$19</c:f>
+              <c:f>'All Comparisons'!$D$19:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1451,15 +1725,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:idx val="6"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$1</c:f>
+              <c:f>'All Comparisons'!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Random Search</c:v>
+                  <c:v>SHA (Sequential)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1467,7 +1741,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1478,11 +1754,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1490,72 +1770,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$B$3:$B$11</c:f>
+              <c:f>'All Comparisons'!$E$28:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.1829504990000004</c:v>
+                  <c:v>7.8567875279999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0321923569999996</c:v>
+                  <c:v>18.032700009999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.175202556999899</c:v>
+                  <c:v>54.981309652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.707698913999899</c:v>
+                  <c:v>130.196151867</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.854793258999997</c:v>
+                  <c:v>316.754186562999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.513741218999996</c:v>
+                  <c:v>638.44272856099997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>173.930542304</c:v>
+                  <c:v>1366.714942757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347.405843667</c:v>
+                  <c:v>3076.4089409479998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>646.110279770999</c:v>
+                  <c:v>6800.0111336159998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14686.297701968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$A$3:$A$11</c:f>
+              <c:f>'All Comparisons'!$A$28:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256</c:v>
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1563,20 +1849,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9F9B-47E1-A228-AD326CCFD2E6}"/>
+              <c16:uniqueId val="{00000000-29CD-4B94-A5D7-BBB668EBAFB2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$22</c:f>
+              <c:f>'All Comparisons'!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SHA</c:v>
+                  <c:v>SHA (4 Workers)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1607,7 +1893,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$E$24:$E$33</c:f>
+              <c:f>'All Comparisons'!$E$44:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1646,7 +1932,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$A$24:$A$33</c:f>
+              <c:f>'All Comparisons'!$A$44:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1692,10 +1978,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$35</c:f>
+              <c:f>'All Comparisons'!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1730,7 +2016,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$37:$F$46</c:f>
+              <c:f>'All Comparisons'!$F$57:$F$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1769,7 +2055,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$H$37:$H$46</c:f>
+              <c:f>'All Comparisons'!$H$57:$H$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1815,10 +2101,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$48</c:f>
+              <c:f>'All Comparisons'!$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1853,7 +2139,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$50:$F$59</c:f>
+              <c:f>'All Comparisons'!$F$70:$F$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1892,7 +2178,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$H$50:$H$59</c:f>
+              <c:f>'All Comparisons'!$H$70:$H$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1938,10 +2224,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Comparisons'!$A$61</c:f>
+              <c:f>'All Comparisons'!$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1976,7 +2262,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$F$63:$F$72</c:f>
+              <c:f>'All Comparisons'!$F$83:$F$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2015,7 +2301,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Comparisons'!$H$63:$H$72</c:f>
+              <c:f>'All Comparisons'!$H$83:$H$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3058,6 +3344,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="745521008"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3818,6 +4105,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="798569888"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3938,7 +4226,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>Accuracy vs. No. of Workers</a:t>
+              <a:t>Accuracy &amp; Runtime vs. No. of Workers</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4575,6 +4863,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="464996000"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -5332,6 +5621,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="798568904"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6070,6 +6360,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="745520024"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -10614,10 +10905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA60ABF5-03AA-4892-B3EE-62DAFC21E578}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10631,1305 +10922,1551 @@
     <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.0610863469999998</v>
+      </c>
+      <c r="B3">
+        <v>0.84380912854934298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>6.1829504990000004</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <v>0.81897465652677304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B8">
         <v>9.0321923569999996</v>
       </c>
-      <c r="C4">
+      <c r="C8">
         <v>0.81897465652677304</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B9">
         <v>14.175202556999899</v>
       </c>
-      <c r="C5">
+      <c r="C9">
         <v>0.82661424571640396</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B10">
         <v>26.707698913999899</v>
       </c>
-      <c r="C6">
+      <c r="C10">
         <v>0.829446683641195</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <v>46.854793258999997</v>
       </c>
-      <c r="C7">
+      <c r="C11">
         <v>0.83464635318708902</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>32</v>
       </c>
-      <c r="B8">
+      <c r="B12">
         <v>90.513741218999996</v>
       </c>
-      <c r="C8">
+      <c r="C12">
         <v>0.83464635318708902</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>64</v>
       </c>
-      <c r="B9">
+      <c r="B13">
         <v>173.930542304</v>
       </c>
-      <c r="C9">
+      <c r="C13">
         <v>0.83990634314602997</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>128</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <v>347.405843667</v>
       </c>
-      <c r="C10">
+      <c r="C14">
         <v>0.84158649364433302</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>256</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <v>646.110279770999</v>
       </c>
-      <c r="C11">
+      <c r="C15">
         <v>0.84158649364433302</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>5.2019904759999998</v>
-      </c>
-      <c r="C15">
-        <v>0.83719238221729497</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>18.543087158999999</v>
-      </c>
-      <c r="C16">
-        <v>0.83695452932256698</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>195.34023031199999</v>
-      </c>
-      <c r="C17">
-        <v>0.84180740610671001</v>
-      </c>
-      <c r="D17">
-        <v>54</v>
+      <c r="A17" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>263.01860896599999</v>
-      </c>
-      <c r="C18">
-        <v>0.84180740610671001</v>
-      </c>
-      <c r="D18">
-        <v>72</v>
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>909.12419303800004</v>
+        <v>5.2019904759999998</v>
       </c>
       <c r="C19">
-        <v>0.84251727493838102</v>
+        <v>0.83719238221729497</v>
       </c>
       <c r="D19">
-        <v>300</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>18.543087158999999</v>
+      </c>
+      <c r="C20">
+        <v>0.83695452932256698</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>195.34023031199999</v>
+      </c>
+      <c r="C21">
+        <v>0.84180740610671001</v>
+      </c>
+      <c r="D21">
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22">
         <v>4</v>
+      </c>
+      <c r="B22">
+        <v>263.01860896599999</v>
+      </c>
+      <c r="C22">
+        <v>0.84180740610671001</v>
+      </c>
+      <c r="D22">
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <v>8.0498952090000007</v>
-      </c>
-      <c r="F24">
-        <v>0.84083328618168596</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25">
-        <v>15.081533</v>
-      </c>
-      <c r="F25">
-        <v>0.84226090624686101</v>
+      <c r="B23">
+        <v>909.12419303800004</v>
+      </c>
+      <c r="C23">
+        <v>0.84251727493838102</v>
+      </c>
+      <c r="D23">
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>37.772597278999903</v>
-      </c>
-      <c r="F26">
-        <v>0.85565691444745295</v>
+      <c r="A26" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>16</v>
-      </c>
-      <c r="D27">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
         <v>2</v>
       </c>
-      <c r="E27">
-        <v>76.902459461999996</v>
-      </c>
-      <c r="F27">
-        <v>0.85839175061064699</v>
+      <c r="F27" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28">
-        <v>163.079588898</v>
+        <v>7.8567875279999999</v>
       </c>
       <c r="F28">
-        <v>0.86131199934760905</v>
+        <v>0.83857121633142395</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29">
-        <v>344.11340940999997</v>
+        <v>18.032700009999999</v>
       </c>
       <c r="F29">
-        <v>0.86440832844621895</v>
+        <v>0.84106500452140698</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>718.65219289300001</v>
+        <v>54.981309652</v>
       </c>
       <c r="F30">
-        <v>0.86622536717754905</v>
+        <v>0.85510070225260804</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>1542.2423894169999</v>
+        <v>130.196151867</v>
       </c>
       <c r="F31">
-        <v>0.86669821754421605</v>
+        <v>0.85827123062081301</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>512</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>512</v>
+        <v>32</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32">
-        <v>3346.5673555899998</v>
+        <v>316.754186562999</v>
       </c>
       <c r="F32">
-        <v>0.86654055228238103</v>
+        <v>0.86166429233839203</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1024</v>
+        <v>64</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1024</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33">
-        <v>7173.2961072520002</v>
+        <v>638.44272856099997</v>
       </c>
       <c r="F33">
-        <v>0.86795896982485299</v>
+        <v>0.86476990517609498</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>15</v>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>128</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>128</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>1366.714942757</v>
+      </c>
+      <c r="F34">
+        <v>0.86679088244786895</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>256</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>256</v>
+      </c>
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="G36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H36" t="s">
-        <v>18</v>
+      <c r="E35">
+        <v>3076.4089409479998</v>
+      </c>
+      <c r="F35">
+        <v>0.86589166383800498</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>512</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>512</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>6800.0111336159998</v>
+      </c>
+      <c r="F36">
+        <v>0.86505731151354803</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>50</v>
+        <v>1024</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1024</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37">
+        <v>14686.297701968</v>
+      </c>
+      <c r="F37">
+        <v>0.86591944234864904</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
         <v>2</v>
       </c>
-      <c r="F37">
-        <v>10.796029871999901</v>
-      </c>
-      <c r="G37">
-        <v>0.85013166666666595</v>
-      </c>
-      <c r="H37">
-        <v>102</v>
+      <c r="F43" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>50</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>2</v>
-      </c>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38">
-        <v>17.55779845</v>
-      </c>
-      <c r="G38">
-        <v>0.85286633333333295</v>
-      </c>
-      <c r="H38">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>50</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>8</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39">
-        <v>8</v>
-      </c>
-      <c r="F39">
-        <v>21.585005923000001</v>
-      </c>
-      <c r="G39">
-        <v>0.855619666666666</v>
-      </c>
-      <c r="H39">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>50</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>16</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40">
-        <v>16</v>
-      </c>
-      <c r="F40">
-        <v>31.505954956</v>
-      </c>
-      <c r="G40">
-        <v>0.855619666666666</v>
-      </c>
-      <c r="H40">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>50</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>32</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41">
-        <v>32</v>
-      </c>
-      <c r="F41">
-        <v>43.335919799999999</v>
-      </c>
-      <c r="G41">
-        <v>0.85816899999999996</v>
-      </c>
-      <c r="H41">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>50</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>64</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42">
-        <v>64</v>
-      </c>
-      <c r="F42">
-        <v>60.480239629000003</v>
-      </c>
-      <c r="G42">
-        <v>0.85968033333333305</v>
-      </c>
-      <c r="H42">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>50</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>128</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43">
-        <v>128</v>
-      </c>
-      <c r="F43">
-        <v>101.41036435300001</v>
-      </c>
-      <c r="G43">
-        <v>0.85968033333333305</v>
-      </c>
-      <c r="H43">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>50</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44">
-        <v>256</v>
+        <v>8.0498952090000007</v>
       </c>
       <c r="F44">
-        <v>191.87340893999999</v>
-      </c>
-      <c r="G44">
-        <v>0.86092266666666595</v>
-      </c>
-      <c r="H44">
-        <v>435</v>
+        <v>0.84083328618168596</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45">
-        <v>512</v>
+        <v>4</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45">
-        <v>512</v>
+        <v>15.081533</v>
       </c>
       <c r="F45">
-        <v>343.72360210599999</v>
-      </c>
-      <c r="G45">
-        <v>0.86092266666666595</v>
-      </c>
-      <c r="H45">
-        <v>489</v>
+        <v>0.84226090624686101</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46">
-        <v>1024</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46">
-        <v>1024</v>
+        <v>37.772597278999903</v>
       </c>
       <c r="F46">
-        <v>683.45206227899996</v>
-      </c>
-      <c r="G46">
-        <v>0.86229466666666599</v>
-      </c>
-      <c r="H46">
-        <v>555</v>
+        <v>0.85565691444745295</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>16</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>76.902459461999996</v>
+      </c>
+      <c r="F47">
+        <v>0.85839175061064699</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>32</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>32</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>163.079588898</v>
+      </c>
+      <c r="F48">
+        <v>0.86131199934760905</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="A49">
+        <v>64</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>64</v>
+      </c>
+      <c r="D49">
         <v>2</v>
       </c>
-      <c r="G49" t="s">
-        <v>3</v>
-      </c>
-      <c r="H49" t="s">
-        <v>18</v>
+      <c r="E49">
+        <v>344.11340940999997</v>
+      </c>
+      <c r="F49">
+        <v>0.86440832844621895</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>200</v>
+        <v>128</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50">
-        <v>2</v>
+        <v>718.65219289300001</v>
       </c>
       <c r="F50">
-        <v>13.9658027069999</v>
-      </c>
-      <c r="G50">
-        <v>0.84925099999999998</v>
-      </c>
-      <c r="H50">
-        <v>228</v>
+        <v>0.86622536717754905</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>1542.2423894169999</v>
       </c>
       <c r="F51">
-        <v>16.405398827999999</v>
-      </c>
-      <c r="G51">
-        <v>0.85287566666666603</v>
-      </c>
-      <c r="H51">
-        <v>578</v>
+        <v>0.86669821754421605</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>200</v>
+        <v>512</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>3346.5673555899998</v>
       </c>
       <c r="F52">
-        <v>22.29913367</v>
-      </c>
-      <c r="G52">
-        <v>0.85461866666666597</v>
-      </c>
-      <c r="H52">
-        <v>728</v>
+        <v>0.86654055228238103</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>200</v>
+        <v>1024</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53">
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53">
-        <v>16</v>
+        <v>7173.2961072520002</v>
       </c>
       <c r="F53">
-        <v>31.990896602999999</v>
-      </c>
-      <c r="G53">
-        <v>0.855619666666666</v>
-      </c>
-      <c r="H53">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>200</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>32</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>32</v>
-      </c>
-      <c r="F54">
-        <v>42.184422892999997</v>
-      </c>
-      <c r="G54">
-        <v>0.85816899999999996</v>
-      </c>
-      <c r="H54">
-        <v>1061</v>
+        <v>0.86795896982485299</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>200</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>64</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-      <c r="E55">
-        <v>64</v>
-      </c>
-      <c r="F55">
-        <v>57.991764947999997</v>
-      </c>
-      <c r="G55">
-        <v>0.86098733333333299</v>
-      </c>
-      <c r="H55">
-        <v>1222</v>
+      <c r="A55" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>200</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>128</v>
-      </c>
-      <c r="D56">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
         <v>2</v>
       </c>
-      <c r="E56">
-        <v>128</v>
-      </c>
-      <c r="F56">
-        <v>88.581890865999995</v>
-      </c>
-      <c r="G56">
-        <v>0.86098733333333299</v>
-      </c>
-      <c r="H56">
-        <v>1403</v>
+      <c r="G56" t="s">
+        <v>3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="F57">
-        <v>155.899168119</v>
+        <v>10.796029871999901</v>
       </c>
       <c r="G57">
-        <v>0.86260999999999999</v>
+        <v>0.85013166666666595</v>
       </c>
       <c r="H57">
-        <v>1604</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58">
-        <v>512</v>
+        <v>4</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
       <c r="E58">
-        <v>512</v>
+        <v>4</v>
       </c>
       <c r="F58">
-        <v>271.48881364300001</v>
+        <v>17.55779845</v>
       </c>
       <c r="G58">
-        <v>0.864408333333333</v>
+        <v>0.85286633333333295</v>
       </c>
       <c r="H58">
-        <v>1808</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59">
-        <v>1024</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <v>2</v>
       </c>
       <c r="E59">
-        <v>1024</v>
+        <v>8</v>
       </c>
       <c r="F59">
-        <v>510.83568611999999</v>
+        <v>21.585005923000001</v>
       </c>
       <c r="G59">
-        <v>0.864408333333333</v>
+        <v>0.855619666666666</v>
       </c>
       <c r="H59">
-        <v>2015</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>50</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>16</v>
+      </c>
+      <c r="F60">
+        <v>31.505954956</v>
+      </c>
+      <c r="G60">
+        <v>0.855619666666666</v>
+      </c>
+      <c r="H60">
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>17</v>
+      <c r="A61">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>32</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>32</v>
+      </c>
+      <c r="F61">
+        <v>43.335919799999999</v>
+      </c>
+      <c r="G61">
+        <v>0.85816899999999996</v>
+      </c>
+      <c r="H61">
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="A62">
+        <v>50</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>64</v>
+      </c>
+      <c r="D62">
         <v>2</v>
       </c>
-      <c r="G62" t="s">
-        <v>3</v>
-      </c>
-      <c r="H62" t="s">
-        <v>18</v>
+      <c r="E62">
+        <v>64</v>
+      </c>
+      <c r="F62">
+        <v>60.480239629000003</v>
+      </c>
+      <c r="G62">
+        <v>0.85968033333333305</v>
+      </c>
+      <c r="H62">
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F63">
-        <v>19.273893206</v>
+        <v>101.41036435300001</v>
       </c>
       <c r="G63">
-        <v>0.85116066666666601</v>
+        <v>0.85968033333333305</v>
       </c>
       <c r="H63">
-        <v>770</v>
+        <v>368</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
       <c r="E64">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="F64">
-        <v>19.343562259999999</v>
+        <v>191.87340893999999</v>
       </c>
       <c r="G64">
-        <v>0.85287566666666603</v>
+        <v>0.86092266666666595</v>
       </c>
       <c r="H64">
-        <v>1339</v>
+        <v>435</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="F65">
-        <v>23.913773534000001</v>
+        <v>343.72360210599999</v>
       </c>
       <c r="G65">
-        <v>0.855619666666666</v>
+        <v>0.86092266666666595</v>
       </c>
       <c r="H65">
-        <v>1772</v>
+        <v>489</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66">
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
       <c r="E66">
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="F66">
-        <v>32.808714103999897</v>
+        <v>683.45206227899996</v>
       </c>
       <c r="G66">
-        <v>0.85609299999999999</v>
+        <v>0.86229466666666599</v>
       </c>
       <c r="H66">
-        <v>2182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>500</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>32</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67">
-        <v>32</v>
-      </c>
-      <c r="F67">
-        <v>45.101742496</v>
-      </c>
-      <c r="G67">
-        <v>0.85816899999999996</v>
-      </c>
-      <c r="H67">
-        <v>2617</v>
+        <v>555</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>500</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68">
-        <v>64</v>
-      </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-      <c r="E68">
-        <v>64</v>
-      </c>
-      <c r="F68">
-        <v>61.014471094000001</v>
-      </c>
-      <c r="G68">
-        <v>0.86098733333333299</v>
-      </c>
-      <c r="H68">
-        <v>3030</v>
+      <c r="A68" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>500</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69">
-        <v>128</v>
-      </c>
-      <c r="D69">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
         <v>2</v>
       </c>
-      <c r="E69">
-        <v>128</v>
-      </c>
-      <c r="F69">
-        <v>90.950749293000001</v>
-      </c>
-      <c r="G69">
-        <v>0.86098733333333299</v>
-      </c>
-      <c r="H69">
-        <v>3472</v>
+      <c r="G69" t="s">
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="F70">
-        <v>158.55057159500001</v>
+        <v>13.9658027069999</v>
       </c>
       <c r="G70">
-        <v>0.86260999999999999</v>
+        <v>0.84925099999999998</v>
       </c>
       <c r="H70">
-        <v>3945</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71">
-        <v>512</v>
+        <v>4</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="E71">
-        <v>512</v>
+        <v>4</v>
       </c>
       <c r="F71">
-        <v>250.56794362400001</v>
+        <v>16.405398827999999</v>
       </c>
       <c r="G71">
-        <v>0.864408333333333</v>
+        <v>0.85287566666666603</v>
       </c>
       <c r="H71">
-        <v>4407</v>
+        <v>578</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72">
-        <v>1024</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>22.29913367</v>
+      </c>
+      <c r="G72">
+        <v>0.85461866666666597</v>
+      </c>
+      <c r="H72">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>200</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>16</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>16</v>
+      </c>
+      <c r="F73">
+        <v>31.990896602999999</v>
+      </c>
+      <c r="G73">
+        <v>0.855619666666666</v>
+      </c>
+      <c r="H73">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>200</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>32</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>32</v>
+      </c>
+      <c r="F74">
+        <v>42.184422892999997</v>
+      </c>
+      <c r="G74">
+        <v>0.85816899999999996</v>
+      </c>
+      <c r="H74">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>200</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>64</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>64</v>
+      </c>
+      <c r="F75">
+        <v>57.991764947999997</v>
+      </c>
+      <c r="G75">
+        <v>0.86098733333333299</v>
+      </c>
+      <c r="H75">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>200</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>128</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>128</v>
+      </c>
+      <c r="F76">
+        <v>88.581890865999995</v>
+      </c>
+      <c r="G76">
+        <v>0.86098733333333299</v>
+      </c>
+      <c r="H76">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>200</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>256</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>256</v>
+      </c>
+      <c r="F77">
+        <v>155.899168119</v>
+      </c>
+      <c r="G77">
+        <v>0.86260999999999999</v>
+      </c>
+      <c r="H77">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>200</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>512</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>512</v>
+      </c>
+      <c r="F78">
+        <v>271.48881364300001</v>
+      </c>
+      <c r="G78">
+        <v>0.864408333333333</v>
+      </c>
+      <c r="H78">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>200</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
         <v>1024</v>
       </c>
-      <c r="F72">
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>1024</v>
+      </c>
+      <c r="F79">
+        <v>510.83568611999999</v>
+      </c>
+      <c r="G79">
+        <v>0.864408333333333</v>
+      </c>
+      <c r="H79">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>2</v>
+      </c>
+      <c r="G82" t="s">
+        <v>3</v>
+      </c>
+      <c r="H82" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>500</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>19.273893206</v>
+      </c>
+      <c r="G83">
+        <v>0.85116066666666601</v>
+      </c>
+      <c r="H83">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>500</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+      <c r="F84">
+        <v>19.343562259999999</v>
+      </c>
+      <c r="G84">
+        <v>0.85287566666666603</v>
+      </c>
+      <c r="H84">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>500</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>8</v>
+      </c>
+      <c r="F85">
+        <v>23.913773534000001</v>
+      </c>
+      <c r="G85">
+        <v>0.855619666666666</v>
+      </c>
+      <c r="H85">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>500</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>16</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <v>16</v>
+      </c>
+      <c r="F86">
+        <v>32.808714103999897</v>
+      </c>
+      <c r="G86">
+        <v>0.85609299999999999</v>
+      </c>
+      <c r="H86">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>500</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>32</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>32</v>
+      </c>
+      <c r="F87">
+        <v>45.101742496</v>
+      </c>
+      <c r="G87">
+        <v>0.85816899999999996</v>
+      </c>
+      <c r="H87">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>500</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>64</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>64</v>
+      </c>
+      <c r="F88">
+        <v>61.014471094000001</v>
+      </c>
+      <c r="G88">
+        <v>0.86098733333333299</v>
+      </c>
+      <c r="H88">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>500</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>128</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>128</v>
+      </c>
+      <c r="F89">
+        <v>90.950749293000001</v>
+      </c>
+      <c r="G89">
+        <v>0.86098733333333299</v>
+      </c>
+      <c r="H89">
+        <v>3472</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>500</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>256</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>256</v>
+      </c>
+      <c r="F90">
+        <v>158.55057159500001</v>
+      </c>
+      <c r="G90">
+        <v>0.86260999999999999</v>
+      </c>
+      <c r="H90">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>500</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>512</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>512</v>
+      </c>
+      <c r="F91">
+        <v>250.56794362400001</v>
+      </c>
+      <c r="G91">
+        <v>0.864408333333333</v>
+      </c>
+      <c r="H91">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>500</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>1024</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>1024</v>
+      </c>
+      <c r="F92">
         <v>467.075928799</v>
       </c>
-      <c r="G72">
+      <c r="G92">
         <v>0.86449166666666599</v>
       </c>
-      <c r="H72">
+      <c r="H92">
         <v>4901</v>
       </c>
     </row>
@@ -11945,7 +12482,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11956,24 +12493,24 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -12168,24 +12705,24 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
         <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
       </c>
       <c r="F13" t="s">
         <v>2</v>
@@ -12403,24 +12940,24 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
         <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -12592,24 +13129,24 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
         <v>9</v>
-      </c>
-      <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
       </c>
       <c r="F39" t="s">
         <v>2</v>
@@ -12827,24 +13364,24 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
         <v>9</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
       </c>
       <c r="F51" t="s">
         <v>2</v>

</xml_diff>